<commit_message>
added year field in the xls file
</commit_message>
<xml_diff>
--- a/public/sample/upload_new_course.xlsx
+++ b/public/sample/upload_new_course.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariful.haque/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC5C11-A1F3-3943-9E5E-47624B0621B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33560" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33555" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>course_code</t>
   </si>
@@ -175,13 +169,19 @@
   </si>
   <si>
     <t>Mat 101</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,9 +210,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -308,7 +309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -485,31 +486,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
     <col min="4" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" customWidth="1"/>
-    <col min="18" max="18" width="30.5" customWidth="1"/>
+    <col min="6" max="6" width="24.125" customWidth="1"/>
+    <col min="9" max="9" width="11" style="2"/>
+    <col min="19" max="19" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -534,53 +536,56 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -605,35 +610,35 @@
       <c r="H2" s="1">
         <v>43328</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J2" s="1">
         <v>43332</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>43363</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>40</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>100</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>5000</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>32</v>
-      </c>
-      <c r="R2" t="s">
-        <v>38</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
@@ -641,8 +646,11 @@
       <c r="T2" t="s">
         <v>38</v>
       </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -667,35 +675,35 @@
       <c r="H3" s="1">
         <v>43328</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="J3" s="1">
         <v>43332</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>43363</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>80</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>100</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>10000</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>33</v>
-      </c>
-      <c r="R3" t="s">
-        <v>39</v>
       </c>
       <c r="S3" t="s">
         <v>39</v>
@@ -703,8 +711,11 @@
       <c r="T3" t="s">
         <v>39</v>
       </c>
+      <c r="U3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -729,35 +740,35 @@
       <c r="H4" s="1">
         <v>43328</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="J4" s="1">
         <v>43332</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>43363</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>120</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>80</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>15000</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>32</v>
-      </c>
-      <c r="R4" t="s">
-        <v>40</v>
       </c>
       <c r="S4" t="s">
         <v>40</v>
@@ -765,8 +776,11 @@
       <c r="T4" t="s">
         <v>40</v>
       </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -791,44 +805,48 @@
       <c r="H5" s="1">
         <v>43328</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
+        <v>2021</v>
+      </c>
+      <c r="J5" s="1">
         <v>43332</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>43363</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>160</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>50</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>26</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>25</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>50000</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>33</v>
-      </c>
-      <c r="R5" t="s">
-        <v>38</v>
       </c>
       <c r="S5" t="s">
         <v>38</v>
       </c>
       <c r="T5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/dev' into traslate"
This reverts commit ec00ed8fd52419764e5cd5d19cf3e29d3d072f69, reversing
changes made to 20fdcc6acfef48eaeefa51d68b42d2c9c8181cae.
</commit_message>
<xml_diff>
--- a/public/sample/upload_new_course.xlsx
+++ b/public/sample/upload_new_course.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariful.haque/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC5C11-A1F3-3943-9E5E-47624B0621B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33555" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33560" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>course_code</t>
   </si>
@@ -169,19 +175,13 @@
   </si>
   <si>
     <t>Mat 101</t>
-  </si>
-  <si>
-    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,10 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -309,7 +308,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -486,32 +485,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="24.125" customWidth="1"/>
-    <col min="9" max="9" width="11" style="2"/>
-    <col min="19" max="19" width="30.5" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="18" max="18" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -536,56 +534,53 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>49</v>
+      <c r="I1" t="s">
+        <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="S1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="W1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -610,35 +605,35 @@
       <c r="H2" s="1">
         <v>43328</v>
       </c>
-      <c r="I2" s="2">
-        <v>2018</v>
+      <c r="I2" s="1">
+        <v>43332</v>
       </c>
       <c r="J2" s="1">
-        <v>43332</v>
-      </c>
-      <c r="K2" s="1">
         <v>43363</v>
       </c>
+      <c r="K2">
+        <v>40</v>
+      </c>
       <c r="L2">
-        <v>40</v>
-      </c>
-      <c r="M2">
         <v>100</v>
       </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
       <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="P2">
+      <c r="O2">
         <v>5000</v>
       </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
@@ -646,11 +641,8 @@
       <c r="T2" t="s">
         <v>38</v>
       </c>
-      <c r="U2" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -675,35 +667,35 @@
       <c r="H3" s="1">
         <v>43328</v>
       </c>
-      <c r="I3" s="2">
-        <v>2019</v>
+      <c r="I3" s="1">
+        <v>43332</v>
       </c>
       <c r="J3" s="1">
-        <v>43332</v>
-      </c>
-      <c r="K3" s="1">
         <v>43363</v>
       </c>
+      <c r="K3">
+        <v>80</v>
+      </c>
       <c r="L3">
-        <v>80</v>
-      </c>
-      <c r="M3">
         <v>100</v>
       </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
       <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="P3">
+      <c r="O3">
         <v>10000</v>
       </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="S3" t="s">
         <v>39</v>
@@ -711,11 +703,8 @@
       <c r="T3" t="s">
         <v>39</v>
       </c>
-      <c r="U3" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -740,35 +729,35 @@
       <c r="H4" s="1">
         <v>43328</v>
       </c>
-      <c r="I4" s="2">
-        <v>2020</v>
+      <c r="I4" s="1">
+        <v>43332</v>
       </c>
       <c r="J4" s="1">
-        <v>43332</v>
-      </c>
-      <c r="K4" s="1">
         <v>43363</v>
       </c>
+      <c r="K4">
+        <v>120</v>
+      </c>
       <c r="L4">
-        <v>120</v>
-      </c>
-      <c r="M4">
         <v>80</v>
       </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
       <c r="N4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="s">
         <v>24</v>
       </c>
-      <c r="P4">
+      <c r="O4">
         <v>15000</v>
       </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
       <c r="Q4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S4" t="s">
         <v>40</v>
@@ -776,11 +765,8 @@
       <c r="T4" t="s">
         <v>40</v>
       </c>
-      <c r="U4" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -805,48 +791,44 @@
       <c r="H5" s="1">
         <v>43328</v>
       </c>
-      <c r="I5" s="2">
-        <v>2021</v>
+      <c r="I5" s="1">
+        <v>43332</v>
       </c>
       <c r="J5" s="1">
-        <v>43332</v>
-      </c>
-      <c r="K5" s="1">
         <v>43363</v>
       </c>
+      <c r="K5">
+        <v>160</v>
+      </c>
       <c r="L5">
-        <v>160</v>
-      </c>
-      <c r="M5">
         <v>50</v>
       </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
       <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
         <v>25</v>
       </c>
-      <c r="P5">
+      <c r="O5">
         <v>50000</v>
       </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
       <c r="Q5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="S5" t="s">
         <v>38</v>
       </c>
       <c r="T5" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>